<commit_message>
Update xlx file to match dataset neighbour
</commit_message>
<xml_diff>
--- a/Toronto-Neighbour-Community.xlsx
+++ b/Toronto-Neighbour-Community.xlsx
@@ -96,9 +96,6 @@
     <t>Clairlea-Birchmount</t>
   </si>
   <si>
-    <t>Wexford-Maryvale</t>
-  </si>
-  <si>
     <t>Tam O'Shanter-Sullivan</t>
   </si>
   <si>
@@ -213,9 +210,6 @@
     <t>Corso Italia-Davenport</t>
   </si>
   <si>
-    <t>Weston-Pelham Park</t>
-  </si>
-  <si>
     <t>Etobicoke York,Etobicoke York,Toronto and East York</t>
   </si>
   <si>
@@ -267,18 +261,12 @@
     <t>Church-Yonge Corridor</t>
   </si>
   <si>
-    <t>North St. James Town</t>
-  </si>
-  <si>
     <t>Moss Park</t>
   </si>
   <si>
     <t>Regent Park</t>
   </si>
   <si>
-    <t>Cabbagetown-South St. James Town</t>
-  </si>
-  <si>
     <t>South Riverdale</t>
   </si>
   <si>
@@ -309,24 +297,15 @@
     <t>East End-Danforth</t>
   </si>
   <si>
-    <t>Taylor-Massey (formerly Crescent Town)</t>
-  </si>
-  <si>
     <t>Woodbine-Lumsden</t>
   </si>
   <si>
-    <t>Danforth - East York</t>
-  </si>
-  <si>
     <t>Old East York</t>
   </si>
   <si>
     <t>Broadview North</t>
   </si>
   <si>
-    <t>Leaside Bennington</t>
-  </si>
-  <si>
     <t>Thorncliffe Park</t>
   </si>
   <si>
@@ -357,9 +336,6 @@
     <t>Pleasant View</t>
   </si>
   <si>
-    <t>Parkwoods Donalda</t>
-  </si>
-  <si>
     <t>Flemingdon Park</t>
   </si>
   <si>
@@ -375,9 +351,6 @@
     <t>Bridle Path-Sunnybrook-York Mills</t>
   </si>
   <si>
-    <t>St. Andrew-Windfields</t>
-  </si>
-  <si>
     <t>Bedford Park-Nortown</t>
   </si>
   <si>
@@ -508,6 +481,33 @@
   </si>
   <si>
     <t>Neighbourhood</t>
+  </si>
+  <si>
+    <t>Wexford/Maryvale</t>
+  </si>
+  <si>
+    <t>Danforth East York</t>
+  </si>
+  <si>
+    <t>North St.James Town</t>
+  </si>
+  <si>
+    <t>Weston-Pellam Park</t>
+  </si>
+  <si>
+    <t>Leaside-Bennington</t>
+  </si>
+  <si>
+    <t>Cabbagetown-South St.James Town</t>
+  </si>
+  <si>
+    <t>Parkwoods-Donalda</t>
+  </si>
+  <si>
+    <t>St.Andrew-Windfields</t>
+  </si>
+  <si>
+    <t>Taylor-Massey</t>
   </si>
 </sst>
 </file>
@@ -887,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -900,1244 +900,1244 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B24" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B26" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B27" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>118</v>
+        <v>161</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B43" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>112</v>
+        <v>160</v>
       </c>
       <c r="B46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B47" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C47" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B50" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C50" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C51" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C52" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B53" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C53" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C54" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C56" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>101</v>
+        <v>158</v>
       </c>
       <c r="C57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B58" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C58" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B59" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C59" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>98</v>
+        <v>155</v>
       </c>
       <c r="C60" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C61" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>96</v>
+        <v>162</v>
       </c>
       <c r="C62" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C63" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B64" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C64" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B65" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C65" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B66" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C66" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B67" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C67" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B68" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C68" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B69" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C69" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B70" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C70" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B71" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C71" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>85</v>
+        <v>159</v>
       </c>
       <c r="B72" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C72" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B73" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C73" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B74" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C74" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
       <c r="B75" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C75" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B76" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C76" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C77" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C78" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B79" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C79" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B80" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C80" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B81" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C81" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B82" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C82" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B83" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C83" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B84" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C84" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B85" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C85" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B86" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C86" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B87" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C87" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B88" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C88" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B89" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C89" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B90" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C90" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B91" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C91" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>64</v>
+        <v>157</v>
       </c>
       <c r="B92" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C92" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B93" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C93" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B94" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C94" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B95" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C95" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B96" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C96" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B97" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C97" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B98" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C98" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B99" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C99" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B100" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C100" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B101" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C101" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B102" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C102" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B103" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C103" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B104" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C104" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B105" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C105" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B106" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C106" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B107" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C107" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B108" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C108" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B109" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C109" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B110" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C110" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B111" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C111" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B112" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C112" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B113" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C113" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B114" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C114" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B115" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C115" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B116" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C116" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B117" t="s">
         <v>0</v>
@@ -2148,7 +2148,7 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B118" t="s">
         <v>5</v>
@@ -2159,7 +2159,7 @@
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B119" t="s">
         <v>5</v>
@@ -2170,7 +2170,7 @@
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>25</v>
+        <v>154</v>
       </c>
       <c r="B120" t="s">
         <v>5</v>

</xml_diff>